<commit_message>
Dokumentation: Kontrolle + Auswertung
- In der Dokumentation Kontrolle und Auswertung fertig geschrieben
- Im Pflichtenheft nachgetragen ob die Vorgaben erfüllt sind
- Kostenkalkulation gemacht
- Terminplan Personen nachgetragen
- Bewertungsbogen weiter abgehakt
</commit_message>
<xml_diff>
--- a/10_Informieren/10_Aufgabenstellung/Bewertungsbogen Pflanzenwagen.xlsx
+++ b/10_Informieren/10_Aufgabenstellung/Bewertungsbogen Pflanzenwagen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE49507-C730-414D-B4F0-67091C99EAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A2E4FF-0D84-4CBC-9F64-008F8EC53455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +432,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1075,7 +1082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1111,9 +1118,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1125,9 +1129,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1317,9 +1318,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1362,6 +1360,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1376,6 +1389,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1769,8 +1785,8 @@
   </sheetPr>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,12 +1803,12 @@
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="41" t="s">
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="39" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1800,22 +1816,22 @@
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="120" t="s">
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="117" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="34" t="s">
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="32" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1824,11 +1840,11 @@
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="42" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="96" t="s">
+      <c r="I3" s="94" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1840,25 +1856,25 @@
         <v>11</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
     </row>
     <row r="5" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="118" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="93">
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="91">
         <v>1</v>
       </c>
     </row>
@@ -1866,31 +1882,31 @@
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="120" t="s">
         <v>104</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="93">
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="118" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="93">
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="91">
         <v>0.5</v>
       </c>
     </row>
@@ -1900,75 +1916,75 @@
         <v>15</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="93">
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
-      <c r="B9" s="124" t="s">
+      <c r="A9" s="104"/>
+      <c r="B9" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110"/>
     </row>
     <row r="10" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="118" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="93">
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="123" t="s">
+      <c r="B11" s="120" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="94">
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="87">
+      <c r="D12" s="53"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="85">
         <f>SUM(H10:H11,H8,H7,H6,H5)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="90">
+      <c r="I12" s="88">
         <f>SUM(I4:I11)</f>
         <v>5</v>
       </c>
@@ -1981,124 +1997,124 @@
         <v>11</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="48"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
     </row>
     <row r="14" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="120" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="93">
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="121" t="s">
+      <c r="B15" s="118" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="93">
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="120" t="s">
         <v>107</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="93">
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="121" t="s">
+      <c r="B17" s="118" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="93">
+      <c r="D17" s="47"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="123" t="s">
+      <c r="B18" s="120" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="93">
+      <c r="D18" s="47"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="118" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="94">
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="92">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="88">
+      <c r="D20" s="53"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="86">
         <f>SUM(H13:H19)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="91">
+      <c r="I20" s="89">
         <f>SUM(I13:I19)</f>
         <v>5</v>
       </c>
@@ -2111,59 +2127,59 @@
         <v>30</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
     </row>
     <row r="22" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="122" t="s">
+      <c r="A22" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="123" t="s">
+      <c r="B22" s="120" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="93">
+      <c r="D22" s="47"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="91">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
-      <c r="B23" s="121" t="s">
+      <c r="B23" s="118" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="94">
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="92">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
-      <c r="C24" s="100" t="s">
+      <c r="C24" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="72"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="88">
+      <c r="D24" s="70"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="86">
         <f>SUM(H22:H23)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="91">
+      <c r="I24" s="89">
         <f>SUM(I21:I23)</f>
         <v>4</v>
       </c>
@@ -2176,12 +2192,12 @@
         <v>35</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="48"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="46"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="81"/>
     </row>
     <row r="26" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
@@ -2189,85 +2205,85 @@
         <v>12</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="93">
+      <c r="D26" s="47"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="122" t="s">
+      <c r="A27" s="119" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
     </row>
     <row r="28" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="123" t="s">
+      <c r="B28" s="120" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="93">
+      <c r="D28" s="47"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="121" t="s">
+      <c r="B29" s="118" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="9"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="93">
+      <c r="D29" s="47"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-      <c r="B30" s="123" t="s">
+      <c r="B30" s="120" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="93">
+      <c r="D30" s="47"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
-      <c r="B31" s="121" t="s">
+      <c r="B31" s="118" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="93">
+      <c r="D31" s="47"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="91">
         <v>0.5</v>
       </c>
     </row>
@@ -2275,61 +2291,61 @@
       <c r="A32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="123" t="s">
+      <c r="B32" s="120" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="10"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="93">
+      <c r="D32" s="47"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="121" t="s">
+      <c r="B33" s="118" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="9"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="93">
+      <c r="D33" s="47"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="123" t="s">
+      <c r="B34" s="120" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="93">
+      <c r="D34" s="47"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
-      <c r="B35" s="125" t="s">
+      <c r="B35" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="93">
+      <c r="C35" s="21"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="91">
         <v>0.5</v>
       </c>
     </row>
@@ -2339,517 +2355,517 @@
         <v>105</v>
       </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="94">
+      <c r="D36" s="51"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="99" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="88">
+      <c r="D37" s="69"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="86">
         <f>SUM(H25:H36)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="91">
+      <c r="I37" s="89">
         <f>SUM(I25:I36)</f>
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="99" t="s">
+      <c r="C38" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="71"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="88">
+      <c r="D38" s="69"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="86">
         <v>0</v>
       </c>
-      <c r="I38" s="91">
+      <c r="I38" s="89">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="128" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C39" s="7"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="64"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="62"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
     </row>
     <row r="40" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="118" t="s">
         <v>48</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="93">
+      <c r="D40" s="47"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="120" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="10"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="93">
+      <c r="D41" s="47"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="118" t="s">
         <v>50</v>
       </c>
       <c r="C42" s="9"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="84"/>
-      <c r="I42" s="84"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="82"/>
     </row>
     <row r="43" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="120"/>
+      <c r="C43" s="124" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="93">
+      <c r="D43" s="47"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="9" t="s">
+      <c r="B44" s="118"/>
+      <c r="C44" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="93">
+      <c r="D44" s="47"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="120"/>
+      <c r="C45" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="49"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="93">
+      <c r="D45" s="47"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="84"/>
-      <c r="I46" s="84"/>
+      <c r="C46" s="125"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82"/>
     </row>
     <row r="47" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="49"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="93">
+      <c r="D47" s="47"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="93">
+      <c r="C48" s="125"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="93">
+      <c r="C49" s="124"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="93">
+      <c r="C50" s="125"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="65"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="94">
+      <c r="C51" s="127"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="63"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="98" t="s">
+      <c r="A52" s="23"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="71"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="88">
+      <c r="D52" s="69"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="86">
         <f>SUM(H39:H51)</f>
         <v>0</v>
       </c>
-      <c r="I52" s="91">
+      <c r="I52" s="89">
         <f>SUM(I39:I51)</f>
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="128" t="s">
         <v>60</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="64"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="62"/>
       <c r="G53" s="18"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="81"/>
     </row>
     <row r="54" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="62"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="93">
+      <c r="C54" s="21"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="62"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="118" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="51"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="84"/>
-      <c r="I55" s="84"/>
+      <c r="C55" s="125"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="82"/>
+      <c r="I55" s="82"/>
     </row>
     <row r="56" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="10" t="s">
+      <c r="B56" s="120"/>
+      <c r="C56" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="49"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="51"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="93">
+      <c r="D56" s="47"/>
+      <c r="E56" s="57"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="9" t="s">
+      <c r="B57" s="118"/>
+      <c r="C57" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="D57" s="49"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="51"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="93">
+      <c r="D57" s="47"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="10" t="s">
+      <c r="B58" s="120"/>
+      <c r="C58" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="D58" s="49"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="51"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="44"/>
-      <c r="I58" s="93">
+      <c r="D58" s="47"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="84"/>
-      <c r="I59" s="84"/>
+      <c r="C59" s="125"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="57"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
     </row>
     <row r="60" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="10" t="s">
+      <c r="B60" s="120"/>
+      <c r="C60" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="D60" s="49"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="93">
+      <c r="D60" s="47"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="9" t="s">
+      <c r="B61" s="118"/>
+      <c r="C61" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="49"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="51"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="93">
+      <c r="D61" s="47"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="120" t="s">
         <v>67</v>
       </c>
       <c r="C62" s="10"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="59"/>
-      <c r="F62" s="51"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="44"/>
-      <c r="I62" s="93">
+      <c r="D62" s="47"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="91">
         <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="118" t="s">
         <v>68</v>
       </c>
       <c r="C63" s="9"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="59"/>
-      <c r="F63" s="51"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="93">
+      <c r="D63" s="47"/>
+      <c r="E63" s="57"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
-      <c r="B64" s="107" t="s">
+      <c r="B64" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="108"/>
-      <c r="D64" s="114"/>
-      <c r="E64" s="115"/>
-      <c r="F64" s="116"/>
-      <c r="G64" s="117"/>
-      <c r="H64" s="118"/>
-      <c r="I64" s="118"/>
+      <c r="C64" s="105"/>
+      <c r="D64" s="111"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="113"/>
+      <c r="G64" s="114"/>
+      <c r="H64" s="115"/>
+      <c r="I64" s="115"/>
     </row>
     <row r="65" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="24"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="98" t="s">
+      <c r="A65" s="23"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="71"/>
-      <c r="E65" s="74"/>
-      <c r="F65" s="73"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="88">
+      <c r="D65" s="69"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="86">
         <f>SUM(H53:H64)</f>
         <v>0</v>
       </c>
-      <c r="I65" s="89">
+      <c r="I65" s="87">
         <f>SUM(I53:I64)</f>
         <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="28" t="s">
         <v>70</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C66" s="17"/>
-      <c r="D66" s="62"/>
-      <c r="E66" s="63"/>
-      <c r="F66" s="64"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="62"/>
       <c r="G66" s="18"/>
-      <c r="H66" s="83"/>
-      <c r="I66" s="83"/>
+      <c r="H66" s="81"/>
+      <c r="I66" s="81"/>
     </row>
     <row r="67" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="120" t="s">
         <v>71</v>
       </c>
       <c r="C67" s="10"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="59"/>
-      <c r="F67" s="51"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="44"/>
-      <c r="I67" s="93">
+      <c r="D67" s="47"/>
+      <c r="E67" s="57"/>
+      <c r="F67" s="49"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="120" t="s">
         <v>72</v>
       </c>
       <c r="C68" s="10"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="59"/>
-      <c r="F68" s="51"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="44"/>
-      <c r="I68" s="93">
+      <c r="D68" s="47"/>
+      <c r="E68" s="57"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="49"/>
-      <c r="E69" s="59"/>
-      <c r="F69" s="51"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="44"/>
-      <c r="I69" s="93">
+      <c r="C69" s="21"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="57"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="91">
         <v>1</v>
       </c>
     </row>
@@ -2859,137 +2875,137 @@
         <v>74</v>
       </c>
       <c r="C70" s="9"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="51"/>
-      <c r="G70" s="35"/>
-      <c r="H70" s="44"/>
-      <c r="I70" s="93">
+      <c r="D70" s="47"/>
+      <c r="E70" s="57"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="42"/>
+      <c r="I70" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="39"/>
+      <c r="A71" s="37"/>
       <c r="B71" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="20"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
-      <c r="F71" s="51"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="44"/>
-      <c r="I71" s="93">
+      <c r="D71" s="49"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="49"/>
+      <c r="G71" s="33"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="31"/>
-      <c r="B72" s="23" t="s">
+      <c r="A72" s="29"/>
+      <c r="B72" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="C72" s="86"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="94">
+      <c r="C72" s="84"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="52"/>
+      <c r="F72" s="52"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="85"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="101" t="s">
+      <c r="A73" s="83"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="73"/>
-      <c r="E73" s="73"/>
-      <c r="F73" s="73"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="88">
+      <c r="D73" s="71"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="86">
         <f>SUM(H67:H72)</f>
         <v>0</v>
       </c>
-      <c r="I73" s="89">
+      <c r="I73" s="87">
         <f>SUM(I67:I72)</f>
         <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
+      <c r="A74" s="129" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="62"/>
-      <c r="E74" s="63"/>
-      <c r="F74" s="64"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="61"/>
+      <c r="F74" s="62"/>
       <c r="G74" s="18"/>
-      <c r="H74" s="83"/>
-      <c r="I74" s="83"/>
+      <c r="H74" s="81"/>
+      <c r="I74" s="81"/>
     </row>
     <row r="75" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="12" t="s">
+      <c r="A75" s="118"/>
+      <c r="B75" s="120" t="s">
         <v>79</v>
       </c>
       <c r="C75" s="10"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="59"/>
-      <c r="F75" s="51"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="93">
+      <c r="D75" s="47"/>
+      <c r="E75" s="57"/>
+      <c r="F75" s="49"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="42"/>
+      <c r="I75" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="12" t="s">
+      <c r="A76" s="119"/>
+      <c r="B76" s="120" t="s">
         <v>80</v>
       </c>
       <c r="C76" s="10"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="35"/>
-      <c r="H76" s="44"/>
-      <c r="I76" s="93">
+      <c r="D76" s="47"/>
+      <c r="E76" s="57"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="11"/>
-      <c r="B77" s="23" t="s">
+      <c r="A77" s="119"/>
+      <c r="B77" s="131" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="15"/>
-      <c r="D77" s="52"/>
-      <c r="E77" s="65"/>
-      <c r="F77" s="54"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="45"/>
-      <c r="I77" s="94"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="52"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="92"/>
     </row>
     <row r="78" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="24"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="102" t="s">
+      <c r="A78" s="23"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="66"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="57"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="88">
+      <c r="D78" s="64"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="55"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="86">
         <f>SUM(H74:H77)</f>
         <v>0</v>
       </c>
-      <c r="I78" s="91">
+      <c r="I78" s="89">
         <f>SUM(I75:I77)</f>
         <v>2</v>
       </c>
@@ -3002,25 +3018,25 @@
         <v>45</v>
       </c>
       <c r="C79" s="17"/>
-      <c r="D79" s="46"/>
-      <c r="E79" s="47"/>
-      <c r="F79" s="48"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="46"/>
       <c r="G79" s="18"/>
-      <c r="H79" s="83"/>
-      <c r="I79" s="83"/>
+      <c r="H79" s="81"/>
+      <c r="I79" s="81"/>
     </row>
     <row r="80" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="120" t="s">
         <v>83</v>
       </c>
       <c r="C80" s="10"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="50"/>
-      <c r="F80" s="51"/>
-      <c r="G80" s="35"/>
-      <c r="H80" s="44"/>
-      <c r="I80" s="93">
+      <c r="D80" s="47"/>
+      <c r="E80" s="48"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="42"/>
+      <c r="I80" s="91">
         <v>0.5</v>
       </c>
     </row>
@@ -3030,29 +3046,29 @@
         <v>84</v>
       </c>
       <c r="C81" s="9"/>
-      <c r="D81" s="53"/>
-      <c r="E81" s="53"/>
-      <c r="F81" s="54"/>
-      <c r="G81" s="37"/>
-      <c r="H81" s="45"/>
-      <c r="I81" s="94">
+      <c r="D81" s="51"/>
+      <c r="E81" s="51"/>
+      <c r="F81" s="52"/>
+      <c r="G81" s="35"/>
+      <c r="H81" s="43"/>
+      <c r="I81" s="92">
         <v>0.5</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="11"/>
-      <c r="C82" s="100" t="s">
+      <c r="C82" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
-      <c r="F82" s="73"/>
-      <c r="G82" s="24"/>
-      <c r="H82" s="88">
+      <c r="D82" s="69"/>
+      <c r="E82" s="69"/>
+      <c r="F82" s="71"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="86">
         <f>SUM(H79:H81)</f>
         <v>0</v>
       </c>
-      <c r="I82" s="91">
+      <c r="I82" s="89">
         <f>SUM(I79:I81)</f>
         <v>1</v>
       </c>
@@ -3065,58 +3081,58 @@
         <v>78</v>
       </c>
       <c r="C83" s="17"/>
-      <c r="D83" s="62"/>
-      <c r="E83" s="75"/>
-      <c r="F83" s="64"/>
+      <c r="D83" s="60"/>
+      <c r="E83" s="73"/>
+      <c r="F83" s="62"/>
       <c r="G83" s="18"/>
-      <c r="H83" s="83"/>
-      <c r="I83" s="83"/>
+      <c r="H83" s="81"/>
+      <c r="I83" s="81"/>
     </row>
     <row r="84" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="120" t="s">
         <v>86</v>
       </c>
       <c r="C84" s="10"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="50"/>
-      <c r="F84" s="51"/>
-      <c r="G84" s="35"/>
-      <c r="H84" s="44"/>
-      <c r="I84" s="93">
+      <c r="D84" s="47"/>
+      <c r="E84" s="48"/>
+      <c r="F84" s="49"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="42"/>
+      <c r="I84" s="91">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="24"/>
-      <c r="B85" s="25" t="s">
+      <c r="A85" s="23"/>
+      <c r="B85" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C85" s="26"/>
-      <c r="D85" s="60"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="61"/>
-      <c r="G85" s="37"/>
-      <c r="H85" s="45"/>
-      <c r="I85" s="94">
+      <c r="C85" s="25"/>
+      <c r="D85" s="58"/>
+      <c r="E85" s="66"/>
+      <c r="F85" s="59"/>
+      <c r="G85" s="35"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11"/>
       <c r="B86" s="3"/>
-      <c r="C86" s="100" t="s">
+      <c r="C86" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="D86" s="66"/>
-      <c r="E86" s="69"/>
-      <c r="F86" s="70"/>
-      <c r="G86" s="24"/>
-      <c r="H86" s="88">
+      <c r="D86" s="64"/>
+      <c r="E86" s="67"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="86">
         <f>SUM(H83:H85)</f>
         <v>0</v>
       </c>
-      <c r="I86" s="91">
+      <c r="I86" s="89">
         <f>SUM(I83:I85)</f>
         <v>2</v>
       </c>
@@ -3129,12 +3145,12 @@
         <v>47</v>
       </c>
       <c r="C87" s="17"/>
-      <c r="D87" s="46"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="48"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="56"/>
+      <c r="F87" s="46"/>
       <c r="G87" s="18"/>
-      <c r="H87" s="83"/>
-      <c r="I87" s="83"/>
+      <c r="H87" s="81"/>
+      <c r="I87" s="81"/>
     </row>
     <row r="88" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
@@ -3142,12 +3158,12 @@
         <v>12</v>
       </c>
       <c r="C88" s="10"/>
-      <c r="D88" s="49"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="51"/>
-      <c r="G88" s="35"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="93">
+      <c r="D88" s="47"/>
+      <c r="E88" s="57"/>
+      <c r="F88" s="49"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="42"/>
+      <c r="I88" s="91">
         <v>2</v>
       </c>
     </row>
@@ -3157,12 +3173,12 @@
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="9"/>
-      <c r="D89" s="49"/>
-      <c r="E89" s="59"/>
-      <c r="F89" s="51"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="44"/>
-      <c r="I89" s="93"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="57"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="91"/>
     </row>
     <row r="90" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
@@ -3170,12 +3186,12 @@
         <v>90</v>
       </c>
       <c r="C90" s="10"/>
-      <c r="D90" s="49"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="51"/>
-      <c r="G90" s="35"/>
-      <c r="H90" s="44"/>
-      <c r="I90" s="93">
+      <c r="D90" s="47"/>
+      <c r="E90" s="57"/>
+      <c r="F90" s="49"/>
+      <c r="G90" s="33"/>
+      <c r="H90" s="42"/>
+      <c r="I90" s="91">
         <v>2</v>
       </c>
     </row>
@@ -3185,12 +3201,12 @@
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="9"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="59"/>
-      <c r="F91" s="51"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="84"/>
-      <c r="I91" s="84"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="57"/>
+      <c r="F91" s="49"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="82"/>
+      <c r="I91" s="82"/>
     </row>
     <row r="92" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
@@ -3198,12 +3214,12 @@
         <v>92</v>
       </c>
       <c r="C92" s="10"/>
-      <c r="D92" s="49"/>
-      <c r="E92" s="59"/>
-      <c r="F92" s="51"/>
-      <c r="G92" s="35"/>
-      <c r="H92" s="44"/>
-      <c r="I92" s="93">
+      <c r="D92" s="47"/>
+      <c r="E92" s="57"/>
+      <c r="F92" s="49"/>
+      <c r="G92" s="33"/>
+      <c r="H92" s="42"/>
+      <c r="I92" s="91">
         <v>1</v>
       </c>
     </row>
@@ -3213,12 +3229,12 @@
         <v>93</v>
       </c>
       <c r="C93" s="9"/>
-      <c r="D93" s="49"/>
-      <c r="E93" s="59"/>
-      <c r="F93" s="51"/>
-      <c r="G93" s="35"/>
-      <c r="H93" s="44"/>
-      <c r="I93" s="93">
+      <c r="D93" s="47"/>
+      <c r="E93" s="57"/>
+      <c r="F93" s="49"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="42"/>
+      <c r="I93" s="91">
         <v>1</v>
       </c>
     </row>
@@ -3228,12 +3244,12 @@
         <v>94</v>
       </c>
       <c r="C94" s="10"/>
-      <c r="D94" s="49"/>
-      <c r="E94" s="59"/>
-      <c r="F94" s="51"/>
-      <c r="G94" s="35"/>
-      <c r="H94" s="44"/>
-      <c r="I94" s="93">
+      <c r="D94" s="47"/>
+      <c r="E94" s="57"/>
+      <c r="F94" s="49"/>
+      <c r="G94" s="33"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="91">
         <v>1</v>
       </c>
     </row>
@@ -3243,12 +3259,12 @@
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="9"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="59"/>
-      <c r="F95" s="51"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="84"/>
-      <c r="I95" s="84"/>
+      <c r="D95" s="47"/>
+      <c r="E95" s="57"/>
+      <c r="F95" s="49"/>
+      <c r="G95" s="33"/>
+      <c r="H95" s="82"/>
+      <c r="I95" s="82"/>
     </row>
     <row r="96" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11"/>
@@ -3256,12 +3272,12 @@
         <v>96</v>
       </c>
       <c r="C96" s="10"/>
-      <c r="D96" s="49"/>
-      <c r="E96" s="59"/>
-      <c r="F96" s="51"/>
-      <c r="G96" s="35"/>
-      <c r="H96" s="44"/>
-      <c r="I96" s="93">
+      <c r="D96" s="47"/>
+      <c r="E96" s="57"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="91">
         <v>1</v>
       </c>
     </row>
@@ -3271,12 +3287,12 @@
         <v>97</v>
       </c>
       <c r="C97" s="9"/>
-      <c r="D97" s="49"/>
-      <c r="E97" s="59"/>
-      <c r="F97" s="51"/>
-      <c r="G97" s="35"/>
-      <c r="H97" s="44"/>
-      <c r="I97" s="93">
+      <c r="D97" s="47"/>
+      <c r="E97" s="57"/>
+      <c r="F97" s="49"/>
+      <c r="G97" s="33"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="91">
         <v>1</v>
       </c>
     </row>
@@ -3286,30 +3302,30 @@
         <v>98</v>
       </c>
       <c r="C98" s="9"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="65"/>
-      <c r="F98" s="54"/>
-      <c r="G98" s="37"/>
-      <c r="H98" s="45"/>
-      <c r="I98" s="94">
+      <c r="D98" s="51"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="52"/>
+      <c r="G98" s="35"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="37"/>
-      <c r="B99" s="23"/>
-      <c r="C99" s="98" t="s">
+      <c r="A99" s="35"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="71"/>
-      <c r="E99" s="74"/>
-      <c r="F99" s="73"/>
-      <c r="G99" s="37"/>
-      <c r="H99" s="88">
+      <c r="D99" s="69"/>
+      <c r="E99" s="72"/>
+      <c r="F99" s="71"/>
+      <c r="G99" s="35"/>
+      <c r="H99" s="86">
         <f>SUM(H87:H98)</f>
         <v>0</v>
       </c>
-      <c r="I99" s="91">
+      <c r="I99" s="89">
         <f>SUM(I87:I98)</f>
         <v>10</v>
       </c>
@@ -3317,38 +3333,38 @@
     <row r="100" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="11"/>
       <c r="B100" s="3"/>
-      <c r="C100" s="103" t="s">
+      <c r="C100" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="D100" s="79"/>
-      <c r="E100" s="80"/>
-      <c r="F100" s="81"/>
-      <c r="G100" s="82"/>
-      <c r="H100" s="104">
+      <c r="D100" s="77"/>
+      <c r="E100" s="78"/>
+      <c r="F100" s="79"/>
+      <c r="G100" s="80"/>
+      <c r="H100" s="102">
         <f>SUM(H99,H86,H82,H78,H73,H65,H52,H38,H37,H24,H20,H12)</f>
         <v>0</v>
       </c>
-      <c r="I100" s="104">
+      <c r="I100" s="102">
         <f>SUM(I99)+I86+I82+I78+I73+I65+I52+I38+I37+I24+I20+I12</f>
         <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A101" s="33" t="s">
+      <c r="A101" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="32" t="s">
+      <c r="B101" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C101" s="77"/>
-      <c r="D101" s="26"/>
-      <c r="E101" s="76"/>
-      <c r="F101" s="78"/>
-      <c r="G101" s="43" t="s">
+      <c r="C101" s="75"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="74"/>
+      <c r="F101" s="76"/>
+      <c r="G101" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="H101" s="92"/>
-      <c r="I101" s="95"/>
+      <c r="H101" s="90"/>
+      <c r="I101" s="93"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
@@ -3360,7 +3376,7 @@
       <c r="G102" s="2"/>
     </row>
     <row r="104" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="G104" s="119" t="s">
+      <c r="G104" s="116" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3405,15 +3421,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010080D5ACB5D9A5C547A8A8A6B4DC26C831" ma:contentTypeVersion="36" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d7a45047883c5514381d1f862dec088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ec5a2d1-872f-46b3-83ae-e3f81ffd97c7" xmlns:ns3="5954586a-bae9-408a-b7c4-5e38477065a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34aeb3f1ae918c8f1a8c56ed432b74e6" ns2:_="" ns3:_="">
     <xsd:import namespace="4ec5a2d1-872f-46b3-83ae-e3f81ffd97c7"/>
@@ -3844,6 +3851,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3901,14 +3917,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A686A6BC-AD03-4242-A509-915B93A7FC06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB0D0B6-0EEB-45DB-9889-96243CF72E68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3927,6 +3935,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A686A6BC-AD03-4242-A509-915B93A7FC06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{753FD138-AAAB-46CD-93E9-84A3CCF0DAEC}">
   <ds:schemaRefs>

</xml_diff>